<commit_message>
se agrego vector de fuerzas locales y globales de resortes
</commit_message>
<xml_diff>
--- a/proyectos/ejemplo1/7/1_elemento.xlsx
+++ b/proyectos/ejemplo1/7/1_elemento.xlsx
@@ -1529,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-16.44564751498782</v>
+        <v>-29.24564751498815</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1537,7 +1537,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-2.04564751498756</v>
+        <v>-27.64564751498822</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1545,7 +1545,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-3.645647514985637</v>
+        <v>-26.04564751498592</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1553,7 +1553,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-5.245647514983045</v>
+        <v>-24.44564751498288</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1561,7 +1561,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-6.845647514983985</v>
+        <v>-22.84564751498458</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1569,7 +1569,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-8.445647514983552</v>
+        <v>-21.2456475149837</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1577,7 +1577,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-10.04564751498828</v>
+        <v>-19.64564751498684</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1585,7 +1585,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-11.64564751498891</v>
+        <v>-18.04564751499014</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1593,7 +1593,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-13.24564751498824</v>
+        <v>-16.44564751498885</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1601,7 +1601,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-14.84564751498592</v>
+        <v>-14.84564751498526</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1609,7 +1609,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-16.44564751498393</v>
+        <v>-13.24564751498398</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1617,7 +1617,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-18.04564751498981</v>
+        <v>-11.64564751498859</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1625,7 +1625,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-19.64564751498782</v>
+        <v>-10.04564751498664</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1633,7 +1633,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-21.24564751498583</v>
+        <v>-8.445647514986666</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1641,7 +1641,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-22.84564751498581</v>
+        <v>-6.845647514987343</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1649,7 +1649,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-24.44564751498906</v>
+        <v>-5.245647514989332</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1657,7 +1657,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-26.04564751498707</v>
+        <v>-3.645647514986078</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1665,7 +1665,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-27.64564751499426</v>
+        <v>-2.04564751499462</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1673,7 +1673,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-13.24564751500322</v>
+        <v>-0.4456475150033954</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1721,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>3420.502055675821</v>
+        <v>4940.502055675838</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1729,7 +1729,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3395.589105376074</v>
+        <v>4371.589105376085</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1737,7 +1737,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>3338.676155076319</v>
+        <v>3834.676155076309</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1745,7 +1745,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>3249.763204776649</v>
+        <v>3329.763204776648</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1753,7 +1753,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>3128.850254476997</v>
+        <v>2856.850254476994</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1761,7 +1761,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>2975.937304177289</v>
+        <v>2415.937304177264</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1769,7 +1769,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2791.024353877654</v>
+        <v>2007.024353877646</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1777,7 +1777,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>2574.111403577758</v>
+        <v>1630.111403577791</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1785,7 +1785,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>2325.198453278098</v>
+        <v>1285.19845327804</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1793,7 +1793,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>2044.285502978229</v>
+        <v>972.285502978237</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1801,7 +1801,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1731.372552678661</v>
+        <v>691.3725526786297</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1809,7 +1809,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1386.459602378871</v>
+        <v>442.4596023788779</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1817,7 +1817,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1009.546652079069</v>
+        <v>225.5466520790862</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1825,7 +1825,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>600.6337017793584</v>
+        <v>40.63370177941211</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1833,7 +1833,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>159.7207514796355</v>
+        <v>-112.2792485203804</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1841,7 +1841,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-313.1921988200739</v>
+        <v>-233.1921988200816</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1849,7 +1849,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-818.1051491199271</v>
+        <v>-322.1051491199537</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1857,7 +1857,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-1355.018099419557</v>
+        <v>-379.0180994195247</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1865,7 +1865,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-1923.931049719698</v>
+        <v>-403.9310497197385</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4185,7 +4185,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.119626442103814e-18</v>
+        <v>1.129851574057469e-18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4193,7 +4193,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.01445650083394892</v>
+        <v>0.02346900992551523</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4201,7 +4201,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.05788603350483316</v>
+        <v>0.08878606467591761</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4209,7 +4209,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1300775752766807</v>
+        <v>0.1911322421300734</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4217,7 +4217,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.23054905050851</v>
+        <v>0.3259596730718583</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4225,7 +4225,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.3585473306543306</v>
+        <v>0.4889915411901583</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4233,7 +4233,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5130482342631429</v>
+        <v>0.6762220830788691</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4241,7 +4241,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.6927565269789372</v>
+        <v>0.8839165882368952</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4249,7 +4249,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.8961059215406948</v>
+        <v>1.108611399068152</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4257,7 +4257,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1.121259077782385</v>
+        <v>1.347113910881561</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4265,7 +4265,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1.366107602632971</v>
+        <v>1.596502571891056</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4273,7 +4273,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1.628272050116403</v>
+        <v>1.854126883215578</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4281,7 +4281,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1.905101921351625</v>
+        <v>2.117607398879081</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4289,7 +4289,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>2.19367566455257</v>
+        <v>2.384835725810527</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4297,7 +4297,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>2.49080067502816</v>
+        <v>2.653974523843885</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4305,7 +4305,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>2.793013295182309</v>
+        <v>2.923457505718136</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4313,7 +4313,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>3.096578814513923</v>
+        <v>3.191989437077271</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4321,7 +4321,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>3.397491469616897</v>
+        <v>3.458546136470289</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -4329,7 +4329,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>3.691474444180114</v>
+        <v>3.722374475351199</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4337,7 +4337,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>3.973979868987453</v>
+        <v>3.982992378079019</v>
       </c>
     </row>
     <row r="22" spans="1:2">

</xml_diff>